<commit_message>
added auth to post
</commit_message>
<xml_diff>
--- a/src/test/resources/PostRooms.xlsx
+++ b/src/test/resources/PostRooms.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>roomId</t>
   </si>
@@ -40,22 +40,40 @@
     <t>expected</t>
   </si>
   <si>
-    <t>"204"</t>
-  </si>
-  <si>
-    <t>"Double"</t>
-  </si>
-  <si>
-    <t>"hiii"</t>
-  </si>
-  <si>
-    <t>"test description"</t>
-  </si>
-  <si>
-    <t>"WiFi, TV"</t>
-  </si>
-  <si>
-    <t>"pass"</t>
+    <t>204</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>hiii</t>
+  </si>
+  <si>
+    <t>Test desc1</t>
+  </si>
+  <si>
+    <t>WiFi|TV</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Test desc</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>Suite</t>
+  </si>
+  <si>
+    <t>not number</t>
   </si>
 </sst>
 </file>
@@ -89,11 +107,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -342,10 +367,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>55.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2">
+        <f t="shared" ref="A2:A5" si="1">VALUE(55)</f>
+        <v>55</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -363,10 +389,104 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1">
-        <v>250.0</v>
+      <c r="H2" s="4">
+        <f t="shared" ref="H2:H5" si="2">VALUE(250)</f>
+        <v>250</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>